<commit_message>
Updated final submission for assignment 4
</commit_message>
<xml_diff>
--- a/Assignment_4_Sampling_techniques.xlsx
+++ b/Assignment_4_Sampling_techniques.xlsx
@@ -8,26 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devansh Dhrafani\Desktop\ML Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF1A559-E2E1-4C1C-8649-AC6E322723C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EA7A04-71C8-496B-8B9C-A76DC8454769}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACCURACY" sheetId="1" r:id="rId1"/>
     <sheet name="FMEASURE" sheetId="2" r:id="rId2"/>
     <sheet name="ANALYSIS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="81">
   <si>
     <t>ACCURACY scores</t>
   </si>
@@ -296,12 +302,6 @@
     <t>Let's look at the Metrics for each technique:</t>
   </si>
   <si>
-    <t xml:space="preserve">Another interesting observation is that if we look at metrics of up-sampled and down-sampled data, accuracy for both is almost the same, </t>
-  </si>
-  <si>
-    <t>but for Down-Sampled data, the F-Measure is higher. This could be due to the fact that when down-sampling, we didn't generate any new data but took the smaller set from</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Let's make a </t>
     </r>
@@ -331,6 +331,94 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alternate Hypothesis</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: "There is significant improvement after applying data sampling techniques".</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Substituting in </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We get Z score of -14.166. For a 95% significance interval, Z-test score is 1.645. As -14.166&lt;1.645, our </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">observations </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>do not</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> lie in the rejection region</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and so</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> H0 is accepted. H1 is rejected.</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>Thus the</t>
     </r>
     <r>
@@ -354,14 +442,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Null Hypothesis: "There is no significant improvement after applying data sampling techniques" is validated.</t>
+      <t>Null Hypothesis H0: "There is no significant improvement after applying data sampling techniques" is validated.</t>
     </r>
   </si>
   <si>
-    <t>Here, we can see that Accuracy/F-Measure of Randomly Sampled dataset is highest. Even after performing different data sampling techniques, accuracy/fmeasure didn't improve,</t>
-  </si>
-  <si>
-    <t>the majority class to balance-out the class imbalance. Thus, our new data was just a class-balanced small subset of original data, and so gave better F-Measure value.</t>
+    <t>Here, we can see that Accuracy/F-Measure of Randomly Sampled dataset is highest. Even after performing different data sampling techniques, accuracy/fmeasure didn't improve.</t>
+  </si>
+  <si>
+    <t>Null Hypothesis is H0: u=0.87 accuracy. Alternate Hypothesis is H1: u&gt;0.87 accuracy. We have x̅ = 0.7, u=0.87, σ=0.127, n=112</t>
   </si>
 </sst>
 </file>
@@ -532,16 +620,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -555,7 +640,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1741,13 +1838,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>302722</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>83128</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>419192</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>34135</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1791,13 +1888,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>272404</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>114299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>430605</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1841,13 +1938,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>295102</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>58883</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>295102</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>142703</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1916,13 +2013,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>378921</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>66502</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>378921</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>150322</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1985,6 +2082,67 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>151384</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9" descr="z score formula">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB02A9CF-9093-4B45-93E9-04CD2E726A60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1097280" y="10066020"/>
+          <a:ext cx="998220" cy="532384"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2253,10 +2411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:T116"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U23" sqref="U23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2269,27 +2427,30 @@
     <col min="7" max="7" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="16"/>
+      <c r="F3" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G3" s="16"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="5" t="s">
         <v>57</v>
@@ -2309,8 +2470,11 @@
       <c r="G4" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -2332,8 +2496,11 @@
       <c r="G5" s="4">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R5" s="14"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="13"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -2355,8 +2522,11 @@
       <c r="G6" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R6" s="14"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="13"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -2378,8 +2548,11 @@
       <c r="G7" s="4">
         <v>0.6875</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R7" s="14"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="13"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -2401,8 +2574,11 @@
       <c r="G8" s="4">
         <v>0.65217400000000003</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R8" s="14"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="13"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -2424,8 +2600,11 @@
       <c r="G9" s="4">
         <v>0.69879500000000005</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R9" s="14"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="13"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -2447,8 +2626,11 @@
       <c r="G10" s="4">
         <v>0.71428599999999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R10" s="14"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="13"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -2470,8 +2652,11 @@
       <c r="G11" s="4">
         <v>0.875</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R11" s="14"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="13"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
@@ -2493,8 +2678,11 @@
       <c r="G12" s="4">
         <v>0.42857099999999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R12" s="14"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="13"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
@@ -2516,8 +2704,11 @@
       <c r="G13" s="4">
         <v>0.50925900000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R13" s="14"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="13"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
@@ -2539,8 +2730,11 @@
       <c r="G14" s="4">
         <v>0.53424700000000003</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R14" s="14"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="13"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
@@ -2562,8 +2756,11 @@
       <c r="G15" s="4">
         <v>0.61702100000000004</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R15" s="14"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="13"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
@@ -2585,8 +2782,11 @@
       <c r="G16" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R16" s="14"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="13"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
@@ -2608,8 +2808,11 @@
       <c r="G17" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R17" s="14"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="13"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
@@ -2631,8 +2834,11 @@
       <c r="G18" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R18" s="14"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="13"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -2654,8 +2860,11 @@
       <c r="G19" s="4">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R19" s="14"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="13"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
@@ -2677,8 +2886,11 @@
       <c r="G20" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R20" s="14"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="13"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
@@ -2700,8 +2912,11 @@
       <c r="G21" s="4">
         <v>0.66666700000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R21" s="14"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="13"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
@@ -2723,8 +2938,11 @@
       <c r="G22" s="4">
         <v>0.68421100000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R22" s="14"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="13"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>19</v>
       </c>
@@ -2746,8 +2964,11 @@
       <c r="G23" s="4">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R23" s="14"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="13"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
@@ -2769,8 +2990,11 @@
       <c r="G24" s="4">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R24" s="14"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="13"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>21</v>
       </c>
@@ -2792,8 +3016,11 @@
       <c r="G25" s="4">
         <v>0.66666700000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R25" s="14"/>
+      <c r="S25" s="15"/>
+      <c r="T25" s="13"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>22</v>
       </c>
@@ -2815,8 +3042,11 @@
       <c r="G26" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R26" s="14"/>
+      <c r="S26" s="15"/>
+      <c r="T26" s="13"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>23</v>
       </c>
@@ -2838,8 +3068,11 @@
       <c r="G27" s="4">
         <v>0.70588200000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R27" s="14"/>
+      <c r="S27" s="15"/>
+      <c r="T27" s="13"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>24</v>
       </c>
@@ -2861,8 +3094,11 @@
       <c r="G28" s="4">
         <v>0.68421100000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R28" s="14"/>
+      <c r="S28" s="15"/>
+      <c r="T28" s="13"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>25</v>
       </c>
@@ -2884,8 +3120,11 @@
       <c r="G29" s="4">
         <v>0.88461500000000004</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R29" s="14"/>
+      <c r="S29" s="15"/>
+      <c r="T29" s="13"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>26</v>
       </c>
@@ -2907,8 +3146,11 @@
       <c r="G30" s="4">
         <v>0.54347800000000002</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R30" s="14"/>
+      <c r="S30" s="15"/>
+      <c r="T30" s="13"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>27</v>
       </c>
@@ -2930,8 +3172,11 @@
       <c r="G31" s="4">
         <v>0.74193500000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R31" s="14"/>
+      <c r="S31" s="15"/>
+      <c r="T31" s="13"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>28</v>
       </c>
@@ -2953,8 +3198,11 @@
       <c r="G32" s="4">
         <v>0.69411800000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R32" s="14"/>
+      <c r="S32" s="15"/>
+      <c r="T32" s="13"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>29</v>
       </c>
@@ -2976,8 +3224,11 @@
       <c r="G33" s="4">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R33" s="14"/>
+      <c r="S33" s="15"/>
+      <c r="T33" s="13"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>30</v>
       </c>
@@ -2999,8 +3250,11 @@
       <c r="G34" s="4">
         <v>0.875</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R34" s="14"/>
+      <c r="S34" s="15"/>
+      <c r="T34" s="13"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>31</v>
       </c>
@@ -3022,8 +3276,11 @@
       <c r="G35" s="4">
         <v>0.70124200000000003</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R35" s="14"/>
+      <c r="S35" s="15"/>
+      <c r="T35" s="13"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>32</v>
       </c>
@@ -3045,8 +3302,11 @@
       <c r="G36" s="4">
         <v>0.75493399999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R36" s="14"/>
+      <c r="S36" s="15"/>
+      <c r="T36" s="13"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>33</v>
       </c>
@@ -3068,8 +3328,11 @@
       <c r="G37" s="4">
         <v>0.63728799999999997</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R37" s="14"/>
+      <c r="S37" s="15"/>
+      <c r="T37" s="13"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>34</v>
       </c>
@@ -3091,8 +3354,11 @@
       <c r="G38" s="4">
         <v>0.65476199999999996</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R38" s="14"/>
+      <c r="S38" s="15"/>
+      <c r="T38" s="13"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>35</v>
       </c>
@@ -3114,8 +3380,11 @@
       <c r="G39" s="4">
         <v>0.58923099999999995</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R39" s="14"/>
+      <c r="S39" s="15"/>
+      <c r="T39" s="13"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>36</v>
       </c>
@@ -3137,8 +3406,11 @@
       <c r="G40" s="4">
         <v>0.60606099999999996</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R40" s="14"/>
+      <c r="S40" s="15"/>
+      <c r="T40" s="13"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>37</v>
       </c>
@@ -3160,8 +3432,11 @@
       <c r="G41" s="4">
         <v>0.71428599999999998</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R41" s="14"/>
+      <c r="S41" s="15"/>
+      <c r="T41" s="13"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>38</v>
       </c>
@@ -3183,8 +3458,11 @@
       <c r="G42" s="4">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R42" s="14"/>
+      <c r="S42" s="15"/>
+      <c r="T42" s="13"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>39</v>
       </c>
@@ -3206,8 +3484,11 @@
       <c r="G43" s="4">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R43" s="14"/>
+      <c r="S43" s="15"/>
+      <c r="T43" s="13"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>40</v>
       </c>
@@ -3229,8 +3510,11 @@
       <c r="G44" s="4">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R44" s="14"/>
+      <c r="S44" s="15"/>
+      <c r="T44" s="13"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>41</v>
       </c>
@@ -3252,8 +3536,11 @@
       <c r="G45" s="4">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R45" s="14"/>
+      <c r="S45" s="15"/>
+      <c r="T45" s="13"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>42</v>
       </c>
@@ -3275,8 +3562,11 @@
       <c r="G46" s="4">
         <v>0.66666700000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R46" s="14"/>
+      <c r="S46" s="15"/>
+      <c r="T46" s="13"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>43</v>
       </c>
@@ -3298,8 +3588,11 @@
       <c r="G47" s="4">
         <v>0.62790699999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R47" s="14"/>
+      <c r="S47" s="15"/>
+      <c r="T47" s="13"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>44</v>
       </c>
@@ -3321,8 +3614,11 @@
       <c r="G48" s="4">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R48" s="14"/>
+      <c r="S48" s="15"/>
+      <c r="T48" s="13"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>45</v>
       </c>
@@ -3344,8 +3640,11 @@
       <c r="G49" s="4">
         <v>0.85714299999999999</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R49" s="14"/>
+      <c r="S49" s="15"/>
+      <c r="T49" s="13"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>46</v>
       </c>
@@ -3367,8 +3666,11 @@
       <c r="G50" s="4">
         <v>0.71428599999999998</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R50" s="14"/>
+      <c r="S50" s="15"/>
+      <c r="T50" s="13"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>47</v>
       </c>
@@ -3390,8 +3692,11 @@
       <c r="G51" s="4">
         <v>0.538462</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R51" s="14"/>
+      <c r="S51" s="15"/>
+      <c r="T51" s="13"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>48</v>
       </c>
@@ -3413,8 +3718,11 @@
       <c r="G52" s="4">
         <v>0.703704</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R52" s="14"/>
+      <c r="S52" s="15"/>
+      <c r="T52" s="13"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>49</v>
       </c>
@@ -3436,8 +3744,11 @@
       <c r="G53" s="4">
         <v>0.58974400000000005</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R53" s="14"/>
+      <c r="S53" s="15"/>
+      <c r="T53" s="13"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>50</v>
       </c>
@@ -3459,8 +3770,11 @@
       <c r="G54" s="4">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R54" s="14"/>
+      <c r="S54" s="15"/>
+      <c r="T54" s="13"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>51</v>
       </c>
@@ -3482,8 +3796,11 @@
       <c r="G55" s="4">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R55" s="14"/>
+      <c r="S55" s="15"/>
+      <c r="T55" s="13"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>52</v>
       </c>
@@ -3505,8 +3822,11 @@
       <c r="G56" s="4">
         <v>0.63888900000000004</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R56" s="14"/>
+      <c r="S56" s="15"/>
+      <c r="T56" s="13"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>53</v>
       </c>
@@ -3528,8 +3848,11 @@
       <c r="G57" s="4">
         <v>0.77142900000000003</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R57" s="14"/>
+      <c r="S57" s="15"/>
+      <c r="T57" s="13"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>54</v>
       </c>
@@ -3551,8 +3874,11 @@
       <c r="G58" s="4">
         <v>0.88435399999999997</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R58" s="14"/>
+      <c r="S58" s="15"/>
+      <c r="T58" s="13"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>55</v>
       </c>
@@ -3574,8 +3900,11 @@
       <c r="G59" s="4">
         <v>0.69230800000000003</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="R59" s="14"/>
+      <c r="S59" s="15"/>
+      <c r="T59" s="13"/>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>56</v>
       </c>
@@ -3597,6 +3926,289 @@
       <c r="G60" s="4">
         <v>0.57142899999999996</v>
       </c>
+      <c r="R60" s="14"/>
+      <c r="S60" s="15"/>
+      <c r="T60" s="13"/>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R61" s="14"/>
+      <c r="S61" s="13"/>
+      <c r="T61" s="13"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R62" s="14"/>
+      <c r="S62" s="13"/>
+      <c r="T62" s="13"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R63" s="14"/>
+      <c r="S63" s="13"/>
+      <c r="T63" s="13"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R64" s="14"/>
+      <c r="S64" s="13"/>
+      <c r="T64" s="13"/>
+    </row>
+    <row r="65" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R65" s="14"/>
+      <c r="S65" s="13"/>
+      <c r="T65" s="13"/>
+    </row>
+    <row r="66" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R66" s="14"/>
+      <c r="S66" s="13"/>
+      <c r="T66" s="13"/>
+    </row>
+    <row r="67" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R67" s="14"/>
+      <c r="S67" s="13"/>
+      <c r="T67" s="13"/>
+    </row>
+    <row r="68" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R68" s="14"/>
+      <c r="S68" s="13"/>
+      <c r="T68" s="13"/>
+    </row>
+    <row r="69" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R69" s="14"/>
+      <c r="S69" s="13"/>
+      <c r="T69" s="13"/>
+    </row>
+    <row r="70" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R70" s="14"/>
+      <c r="S70" s="13"/>
+      <c r="T70" s="13"/>
+    </row>
+    <row r="71" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R71" s="14"/>
+      <c r="S71" s="13"/>
+      <c r="T71" s="13"/>
+    </row>
+    <row r="72" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R72" s="14"/>
+      <c r="S72" s="13"/>
+      <c r="T72" s="13"/>
+    </row>
+    <row r="73" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R73" s="14"/>
+      <c r="S73" s="13"/>
+      <c r="T73" s="13"/>
+    </row>
+    <row r="74" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R74" s="14"/>
+      <c r="S74" s="13"/>
+      <c r="T74" s="13"/>
+    </row>
+    <row r="75" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R75" s="14"/>
+      <c r="S75" s="13"/>
+      <c r="T75" s="13"/>
+    </row>
+    <row r="76" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R76" s="14"/>
+      <c r="S76" s="13"/>
+      <c r="T76" s="13"/>
+    </row>
+    <row r="77" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R77" s="14"/>
+      <c r="S77" s="13"/>
+      <c r="T77" s="13"/>
+    </row>
+    <row r="78" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R78" s="14"/>
+      <c r="S78" s="13"/>
+      <c r="T78" s="13"/>
+    </row>
+    <row r="79" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R79" s="14"/>
+      <c r="S79" s="13"/>
+      <c r="T79" s="13"/>
+    </row>
+    <row r="80" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R80" s="14"/>
+      <c r="S80" s="13"/>
+      <c r="T80" s="13"/>
+    </row>
+    <row r="81" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R81" s="14"/>
+      <c r="S81" s="13"/>
+      <c r="T81" s="13"/>
+    </row>
+    <row r="82" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R82" s="14"/>
+      <c r="S82" s="13"/>
+      <c r="T82" s="13"/>
+    </row>
+    <row r="83" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R83" s="14"/>
+      <c r="S83" s="13"/>
+      <c r="T83" s="13"/>
+    </row>
+    <row r="84" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R84" s="14"/>
+      <c r="S84" s="13"/>
+      <c r="T84" s="13"/>
+    </row>
+    <row r="85" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R85" s="14"/>
+      <c r="S85" s="13"/>
+      <c r="T85" s="13"/>
+    </row>
+    <row r="86" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R86" s="14"/>
+      <c r="S86" s="13"/>
+      <c r="T86" s="13"/>
+    </row>
+    <row r="87" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R87" s="14"/>
+      <c r="S87" s="13"/>
+      <c r="T87" s="13"/>
+    </row>
+    <row r="88" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R88" s="14"/>
+      <c r="S88" s="13"/>
+      <c r="T88" s="13"/>
+    </row>
+    <row r="89" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R89" s="14"/>
+      <c r="S89" s="13"/>
+      <c r="T89" s="13"/>
+    </row>
+    <row r="90" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R90" s="14"/>
+      <c r="S90" s="13"/>
+      <c r="T90" s="13"/>
+    </row>
+    <row r="91" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R91" s="14"/>
+      <c r="S91" s="13"/>
+      <c r="T91" s="13"/>
+    </row>
+    <row r="92" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R92" s="14"/>
+      <c r="S92" s="13"/>
+      <c r="T92" s="13"/>
+    </row>
+    <row r="93" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R93" s="14"/>
+      <c r="S93" s="13"/>
+      <c r="T93" s="13"/>
+    </row>
+    <row r="94" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R94" s="14"/>
+      <c r="S94" s="13"/>
+      <c r="T94" s="13"/>
+    </row>
+    <row r="95" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R95" s="14"/>
+      <c r="S95" s="13"/>
+      <c r="T95" s="13"/>
+    </row>
+    <row r="96" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R96" s="14"/>
+      <c r="S96" s="13"/>
+      <c r="T96" s="13"/>
+    </row>
+    <row r="97" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R97" s="14"/>
+      <c r="S97" s="13"/>
+      <c r="T97" s="13"/>
+    </row>
+    <row r="98" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R98" s="14"/>
+      <c r="S98" s="13"/>
+      <c r="T98" s="13"/>
+    </row>
+    <row r="99" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R99" s="14"/>
+      <c r="S99" s="13"/>
+      <c r="T99" s="13"/>
+    </row>
+    <row r="100" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R100" s="14"/>
+      <c r="S100" s="13"/>
+      <c r="T100" s="13"/>
+    </row>
+    <row r="101" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R101" s="14"/>
+      <c r="S101" s="13"/>
+      <c r="T101" s="13"/>
+    </row>
+    <row r="102" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R102" s="14"/>
+      <c r="S102" s="13"/>
+      <c r="T102" s="13"/>
+    </row>
+    <row r="103" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R103" s="14"/>
+      <c r="S103" s="13"/>
+      <c r="T103" s="13"/>
+    </row>
+    <row r="104" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R104" s="14"/>
+      <c r="S104" s="13"/>
+      <c r="T104" s="13"/>
+    </row>
+    <row r="105" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R105" s="14"/>
+      <c r="S105" s="13"/>
+      <c r="T105" s="13"/>
+    </row>
+    <row r="106" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R106" s="14"/>
+      <c r="S106" s="13"/>
+      <c r="T106" s="13"/>
+    </row>
+    <row r="107" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R107" s="14"/>
+      <c r="S107" s="13"/>
+      <c r="T107" s="13"/>
+    </row>
+    <row r="108" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R108" s="14"/>
+      <c r="S108" s="13"/>
+      <c r="T108" s="13"/>
+    </row>
+    <row r="109" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R109" s="14"/>
+      <c r="S109" s="13"/>
+      <c r="T109" s="13"/>
+    </row>
+    <row r="110" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R110" s="14"/>
+      <c r="S110" s="13"/>
+      <c r="T110" s="13"/>
+    </row>
+    <row r="111" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R111" s="14"/>
+      <c r="S111" s="13"/>
+      <c r="T111" s="13"/>
+    </row>
+    <row r="112" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R112" s="14"/>
+      <c r="S112" s="13"/>
+      <c r="T112" s="13"/>
+    </row>
+    <row r="113" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R113" s="14"/>
+      <c r="S113" s="13"/>
+      <c r="T113" s="13"/>
+    </row>
+    <row r="114" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R114" s="14"/>
+      <c r="S114" s="13"/>
+      <c r="T114" s="13"/>
+    </row>
+    <row r="115" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R115" s="14"/>
+      <c r="S115" s="13"/>
+      <c r="T115" s="13"/>
+    </row>
+    <row r="116" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R116" s="14"/>
+      <c r="S116" s="13"/>
+      <c r="T116" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3615,8 +4227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9BD595-47B5-4C5E-ACEA-FF919BC9447D}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T30" sqref="T30"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3631,43 +4243,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="10"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="16"/>
+      <c r="F3" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>58</v>
       </c>
     </row>
@@ -4973,10 +5585,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B27EB781-D146-4A6F-A2F5-274544BB91DE}">
-  <dimension ref="A1:R55"/>
+  <dimension ref="A1:S63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:R60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4985,328 +5597,479 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
     </row>
     <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
     </row>
     <row r="23" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
     </row>
     <row r="24" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
     </row>
     <row r="25" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
     </row>
     <row r="26" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
     </row>
     <row r="27" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
+    </row>
+    <row r="28" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="12"/>
+    </row>
+    <row r="30" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+    </row>
+    <row r="52" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" s="18"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="18"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="18"/>
+      <c r="M52" s="18"/>
+      <c r="N52" s="18"/>
+      <c r="O52" s="18"/>
+      <c r="P52" s="18"/>
+      <c r="Q52" s="18"/>
+      <c r="R52" s="18"/>
+    </row>
+    <row r="53" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="18"/>
+      <c r="N53" s="18"/>
+      <c r="O53" s="18"/>
+      <c r="P53" s="18"/>
+      <c r="Q53" s="18"/>
+      <c r="R53" s="18"/>
+    </row>
+    <row r="54" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-    </row>
-    <row r="29" spans="1:18" ht="18" x14ac:dyDescent="0.35">
-      <c r="A29" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-    </row>
-    <row r="32" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-    </row>
-    <row r="50" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="13" t="s">
+      <c r="B54" s="18"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="18"/>
+      <c r="J54" s="18"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="18"/>
+      <c r="M54" s="18"/>
+      <c r="N54" s="18"/>
+      <c r="O54" s="18"/>
+      <c r="P54" s="18"/>
+      <c r="Q54" s="18"/>
+      <c r="R54" s="18"/>
+    </row>
+    <row r="55" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="18"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
+      <c r="J55" s="18"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="18"/>
+      <c r="M55" s="18"/>
+      <c r="N55" s="18"/>
+      <c r="O55" s="18"/>
+      <c r="P55" s="18"/>
+      <c r="Q55" s="18"/>
+      <c r="R55" s="18"/>
+    </row>
+    <row r="56" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="18"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+      <c r="I56" s="18"/>
+      <c r="J56" s="18"/>
+      <c r="K56" s="18"/>
+      <c r="L56" s="18"/>
+      <c r="M56" s="18"/>
+      <c r="N56" s="18"/>
+      <c r="O56" s="18"/>
+      <c r="P56" s="18"/>
+      <c r="Q56" s="18"/>
+      <c r="R56" s="18"/>
+    </row>
+    <row r="57" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" s="18"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+      <c r="J57" s="18"/>
+      <c r="K57" s="18"/>
+      <c r="L57" s="18"/>
+      <c r="M57" s="18"/>
+      <c r="N57" s="18"/>
+      <c r="O57" s="18"/>
+      <c r="P57" s="18"/>
+      <c r="Q57" s="18"/>
+      <c r="R57" s="18"/>
+      <c r="S57" s="18"/>
+    </row>
+    <row r="58" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="18"/>
+      <c r="B58" s="18"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="18"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18"/>
+      <c r="L58" s="18"/>
+      <c r="M58" s="18"/>
+      <c r="N58" s="18"/>
+      <c r="O58" s="18"/>
+      <c r="P58" s="18"/>
+      <c r="Q58" s="18"/>
+      <c r="R58" s="18"/>
+    </row>
+    <row r="59" spans="1:19" ht="18" x14ac:dyDescent="0.3">
+      <c r="A59" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B50" s="13"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13"/>
-      <c r="K50" s="13"/>
-      <c r="L50" s="13"/>
-      <c r="M50" s="13"/>
-      <c r="N50" s="13"/>
-      <c r="O50" s="13"/>
-      <c r="P50" s="13"/>
-      <c r="Q50" s="13"/>
-      <c r="R50" s="13"/>
-    </row>
-    <row r="51" spans="1:18" ht="18" x14ac:dyDescent="0.3">
-      <c r="A51" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="14"/>
-      <c r="M51" s="14"/>
-      <c r="N51" s="14"/>
-      <c r="O51" s="14"/>
-      <c r="P51" s="14"/>
-      <c r="Q51" s="14"/>
-      <c r="R51" s="14"/>
-    </row>
-    <row r="52" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="13"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="13"/>
-      <c r="J52" s="13"/>
-      <c r="K52" s="13"/>
-      <c r="L52" s="13"/>
-      <c r="M52" s="13"/>
-      <c r="N52" s="13"/>
-      <c r="O52" s="13"/>
-      <c r="P52" s="13"/>
-      <c r="Q52" s="13"/>
-      <c r="R52" s="13"/>
-    </row>
-    <row r="53" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="B53" s="13"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="13"/>
-      <c r="J53" s="13"/>
-      <c r="K53" s="13"/>
-      <c r="L53" s="13"/>
-      <c r="M53" s="13"/>
-      <c r="N53" s="13"/>
-      <c r="O53" s="13"/>
-      <c r="P53" s="13"/>
-      <c r="Q53" s="13"/>
-      <c r="R53" s="13"/>
-    </row>
-    <row r="54" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B54" s="13"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="13"/>
-      <c r="I54" s="13"/>
-      <c r="J54" s="13"/>
-      <c r="K54" s="13"/>
-      <c r="L54" s="13"/>
-      <c r="M54" s="13"/>
-      <c r="N54" s="13"/>
-      <c r="O54" s="13"/>
-      <c r="P54" s="13"/>
-      <c r="Q54" s="13"/>
-      <c r="R54" s="13"/>
-    </row>
-    <row r="55" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B55" s="13"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="13"/>
-      <c r="I55" s="13"/>
-      <c r="J55" s="13"/>
-      <c r="K55" s="13"/>
-      <c r="L55" s="13"/>
-      <c r="M55" s="13"/>
-      <c r="N55" s="13"/>
-      <c r="O55" s="13"/>
-      <c r="P55" s="13"/>
-      <c r="Q55" s="13"/>
-      <c r="R55" s="13"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+      <c r="J59" s="17"/>
+      <c r="K59" s="17"/>
+      <c r="L59" s="17"/>
+      <c r="M59" s="17"/>
+      <c r="N59" s="17"/>
+      <c r="O59" s="17"/>
+      <c r="P59" s="17"/>
+      <c r="Q59" s="17"/>
+      <c r="R59" s="17"/>
+    </row>
+    <row r="60" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="18"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
+      <c r="J60" s="18"/>
+      <c r="K60" s="18"/>
+      <c r="L60" s="18"/>
+      <c r="M60" s="18"/>
+      <c r="N60" s="18"/>
+      <c r="O60" s="18"/>
+      <c r="P60" s="18"/>
+      <c r="Q60" s="18"/>
+      <c r="R60" s="18"/>
+    </row>
+    <row r="61" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="18"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="18"/>
+      <c r="L61" s="18"/>
+      <c r="M61" s="18"/>
+      <c r="N61" s="18"/>
+      <c r="O61" s="18"/>
+      <c r="P61" s="18"/>
+      <c r="Q61" s="18"/>
+      <c r="R61" s="18"/>
+    </row>
+    <row r="62" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="18"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="18"/>
+      <c r="I62" s="18"/>
+      <c r="J62" s="18"/>
+      <c r="K62" s="18"/>
+      <c r="L62" s="18"/>
+      <c r="M62" s="18"/>
+      <c r="N62" s="18"/>
+      <c r="O62" s="18"/>
+      <c r="P62" s="18"/>
+      <c r="Q62" s="18"/>
+      <c r="R62" s="18"/>
+    </row>
+    <row r="63" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="18"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18"/>
+      <c r="I63" s="18"/>
+      <c r="J63" s="18"/>
+      <c r="K63" s="18"/>
+      <c r="L63" s="18"/>
+      <c r="M63" s="18"/>
+      <c r="N63" s="18"/>
+      <c r="O63" s="18"/>
+      <c r="P63" s="18"/>
+      <c r="Q63" s="18"/>
+      <c r="R63" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A51:R51"/>
-    <mergeCell ref="A52:R52"/>
+  <mergeCells count="22">
     <mergeCell ref="A53:R53"/>
+    <mergeCell ref="A58:R58"/>
     <mergeCell ref="A54:R54"/>
     <mergeCell ref="A55:R55"/>
+    <mergeCell ref="A56:R56"/>
+    <mergeCell ref="A57:S57"/>
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A31:L31"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A50:R50"/>
+    <mergeCell ref="A32:L32"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="A52:R52"/>
     <mergeCell ref="A25:R25"/>
     <mergeCell ref="A24:R24"/>
     <mergeCell ref="A23:R23"/>
     <mergeCell ref="A26:R26"/>
     <mergeCell ref="A27:R27"/>
+    <mergeCell ref="A28:Q28"/>
+    <mergeCell ref="A59:R59"/>
+    <mergeCell ref="A60:R60"/>
+    <mergeCell ref="A61:R61"/>
+    <mergeCell ref="A62:R62"/>
+    <mergeCell ref="A63:R63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>